<commit_message>
Preparing for Cappy edits to NESSF18 proposal.
</commit_message>
<xml_diff>
--- a/doc/proposals/NESSF18/budget/budget.xlsx
+++ b/doc/proposals/NESSF18/budget/budget.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t xml:space="preserve">Category</t>
   </si>
@@ -28,43 +28,37 @@
     <t xml:space="preserve"> Item</t>
   </si>
   <si>
-    <t xml:space="preserve">6 credits per semester</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 credits per year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Cost</t>
+    <t xml:space="preserve">Cost</t>
   </si>
   <si>
     <t xml:space="preserve">University Enrollment</t>
   </si>
   <si>
-    <t xml:space="preserve">Tuition/Fees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gym Fee</t>
+    <t xml:space="preserve">Tuition/Fees (1 year)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gym Fee (1 year)</t>
   </si>
   <si>
     <t xml:space="preserve">Insurance</t>
   </si>
   <si>
-    <t xml:space="preserve">Heath</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dental</t>
+    <t xml:space="preserve">Heath (1 year)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dental (1 year)</t>
   </si>
   <si>
     <t xml:space="preserve">Conferences</t>
   </si>
   <si>
-    <t xml:space="preserve">Airfare (2x national average)</t>
+    <t xml:space="preserve">Meals (week @ per diem rate)</t>
   </si>
   <si>
     <t xml:space="preserve">Lodging (week @ per diem rate)</t>
   </si>
   <si>
-    <t xml:space="preserve">Meals (week @ per diem rate)</t>
+    <t xml:space="preserve">Airfare (remainder)</t>
   </si>
   <si>
     <t xml:space="preserve">Stipend</t>
@@ -172,20 +166,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.4489795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.2857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.9489795918367"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -198,148 +192,107 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>1887</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <f aca="false">2 *C2</f>
+        <f aca="false">2*1887</f>
         <v>3774</v>
       </c>
-      <c r="E2" s="1" t="n">
-        <f aca="false">D2</f>
-        <v>3774</v>
-      </c>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>78.75</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <f aca="false">2 *C3</f>
+        <f aca="false">2*78.75</f>
         <v>157.5</v>
       </c>
-      <c r="E3" s="1" t="n">
-        <f aca="false">D3</f>
-        <v>157.5</v>
-      </c>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>2000.92</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <f aca="false">2 *C4</f>
+        <f aca="false">2*2000.92</f>
         <v>4001.84</v>
       </c>
-      <c r="E4" s="1" t="n">
-        <f aca="false">D4</f>
-        <v>4001.84</v>
-      </c>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>220.25</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <f aca="false">2 *C5</f>
+        <f aca="false">2*220.25</f>
         <v>440.5</v>
       </c>
-      <c r="E5" s="1" t="n">
-        <f aca="false">D5</f>
-        <v>440.5</v>
-      </c>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <f aca="false">46*7</f>
+        <v>322</v>
+      </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="1" t="n">
-        <f aca="false">354*2</f>
-        <v>708</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="n">
         <f aca="false">7*93</f>
         <v>651</v>
       </c>
+      <c r="D7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <f aca="false">354*2 - 54.84</f>
+        <v>653.16</v>
+      </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="1" t="n">
-        <f aca="false">46*7</f>
-        <v>322</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>35000</v>
+      </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="1" t="n">
-        <v>35000</v>
-      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1" t="n">
         <f aca="false">SUM(C2:C9)</f>
-        <v>4186.92</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <f aca="false">SUM(D2:D9)</f>
-        <v>8373.84</v>
-      </c>
-      <c r="E10" s="1" t="n">
-        <f aca="false">SUM(E2:E9)</f>
-        <v>45054.84</v>
-      </c>
+        <v>45000</v>
+      </c>
+      <c r="D10" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>